<commit_message>
make goslim pie font bigger
</commit_message>
<xml_diff>
--- a/analyses/make_GOslim-pie.xlsx
+++ b/analyses/make_GOslim-pie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5615BF-6D5C-A048-9470-36B4F66AED93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9019C-61CC-1543-8F0A-69DDB33D69CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{FE4F1217-DAFC-2E42-B740-2F7A2F21ACD8}"/>
   </bookViews>
@@ -445,10 +445,76 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-5330-8E44-85B2-39443352CC5B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0693352479395241E-2"/>
+                  <c:y val="9.6852300242130755E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.17426520064795967"/>
+                      <c:h val="0.11937046004842615"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-48EA-A84A-9F89-C4A4D80DC88A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6578749058025512E-2"/>
+                  <c:y val="1.6949152542372881E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -463,9 +529,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent1"/>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -475,7 +541,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -483,21 +549,20 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="9.7400091378931797E-2"/>
-                      <c:h val="7.8208232445520567E-2"/>
-                    </c:manualLayout>
-                  </c15:layout>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-48EA-A84A-9F89-C4A4D80DC88A}"/>
+                  <c16:uniqueId val="{00000006-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="1"/>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0550113036925506E-2"/>
+                  <c:y val="-5.8111380145278495E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -512,9 +577,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent3"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -524,7 +589,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -532,13 +597,20 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-48EA-A84A-9F89-C4A4D80DC88A}"/>
+                  <c16:uniqueId val="{00000007-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="2"/>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.562170308967596E-2"/>
+                  <c:y val="-1.2106537530266344E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -553,9 +625,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent3"/>
+                        <a:schemeClr val="accent4"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -565,7 +637,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -573,13 +645,75 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-48EA-A84A-9F89-C4A4D80DC88A}"/>
+                  <c16:uniqueId val="{00000008-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="3"/>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.6578749058025623E-2"/>
+                  <c:y val="-3.7530266343825648E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.25331141821288916"/>
+                      <c:h val="0.16703361232388328"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-48EA-A84A-9F89-C4A4D80DC88A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.5610547739558069E-2"/>
+                  <c:y val="3.5716001601494726E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -594,103 +728,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="accent4"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-48EA-A84A-9F89-C4A4D80DC88A}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.19905364131273873"/>
-                      <c:h val="0.12587131367292223"/>
-                    </c:manualLayout>
-                  </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-48EA-A84A-9F89-C4A4D80DC88A}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.4100596760443308E-3"/>
-                  <c:y val="1.8766756032171483E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent6"/>
                       </a:solidFill>
@@ -738,7 +776,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent1">
                           <a:lumMod val="60000"/>
@@ -768,6 +806,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.9186134137151468E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -782,7 +826,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent2">
                           <a:lumMod val="60000"/>
@@ -796,7 +840,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -804,6 +848,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
@@ -811,6 +856,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3564431047475515E-2"/>
+                  <c:y val="-2.4213075060532689E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -825,7 +876,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent3">
                           <a:lumMod val="60000"/>
@@ -839,7 +890,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -847,6 +898,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
@@ -863,12 +915,12 @@
               </c:spPr>
               <c:txPr>
                 <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
+                  <a:noAutofit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent4">
                           <a:lumMod val="60000"/>
@@ -890,6 +942,14 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.17274308872656929"/>
+                      <c:h val="0.17092009685230025"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
@@ -897,6 +957,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3564431047475508E-2"/>
+                  <c:y val="7.2639225181598066E-3"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -911,7 +977,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent5">
                           <a:lumMod val="60000"/>
@@ -925,7 +991,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -933,6 +999,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-48EA-A84A-9F89-C4A4D80DC88A}"/>
                 </c:ext>
@@ -960,7 +1027,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent6">
                           <a:lumMod val="60000"/>
@@ -983,8 +1050,18 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-5330-8E44-85B2-39443352CC5B}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
@@ -992,7 +1069,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="accent1"/>
                     </a:solidFill>

</xml_diff>

<commit_message>
save new color scheme for pie
</commit_message>
<xml_diff>
--- a/analyses/make_GOslim-pie.xlsx
+++ b/analyses/make_GOslim-pie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9019C-61CC-1543-8F0A-69DDB33D69CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7681C173-E37E-9648-BEA8-7ADA58C8EAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{FE4F1217-DAFC-2E42-B740-2F7A2F21ACD8}"/>
   </bookViews>
@@ -156,7 +156,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -180,7 +180,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -204,7 +204,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -228,7 +228,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -252,7 +254,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -276,7 +280,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -300,8 +306,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -326,8 +333,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -352,8 +360,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -378,8 +387,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -404,8 +413,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -431,7 +440,7 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
+                  <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -476,7 +485,7 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent1"/>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -531,7 +540,7 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent4"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -579,7 +588,7 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent3"/>
+                        <a:schemeClr val="accent6"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -627,7 +636,9 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent4"/>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -675,7 +686,9 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent5"/>
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -730,7 +743,9 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6"/>
+                        <a:schemeClr val="accent6">
+                          <a:lumMod val="60000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -778,8 +793,9 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent1">
-                          <a:lumMod val="60000"/>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="80000"/>
+                          <a:lumOff val="20000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -828,8 +844,9 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2">
-                          <a:lumMod val="60000"/>
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="80000"/>
+                          <a:lumOff val="20000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -878,8 +895,9 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent3">
-                          <a:lumMod val="60000"/>
+                        <a:schemeClr val="accent6">
+                          <a:lumMod val="80000"/>
+                          <a:lumOff val="20000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -922,8 +940,8 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent4">
-                          <a:lumMod val="60000"/>
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="80000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -979,8 +997,8 @@
                   <a:pPr>
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent5">
-                          <a:lumMod val="60000"/>
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="80000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -1030,7 +1048,7 @@
                     <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="accent6">
-                          <a:lumMod val="60000"/>
+                          <a:lumMod val="80000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
@@ -1267,12 +1285,9 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>

</xml_diff>

<commit_message>
save color change and bigger font
</commit_message>
<xml_diff>
--- a/analyses/make_GOslim-pie.xlsx
+++ b/analyses/make_GOslim-pie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graciecrandall/Documents/GitHub/project-crab/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7681C173-E37E-9648-BEA8-7ADA58C8EAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CCA630-EE2E-9C44-A471-5A5537FCD99F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{FE4F1217-DAFC-2E42-B740-2F7A2F21ACD8}"/>
   </bookViews>
@@ -156,7 +156,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -180,7 +180,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -204,7 +204,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -228,7 +228,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent6">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -254,7 +254,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent5">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -280,7 +280,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
+                <a:schemeClr val="accent4">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -306,7 +306,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent6">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
@@ -333,7 +333,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent5">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
@@ -360,7 +360,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
+                <a:schemeClr val="accent4">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
@@ -387,7 +387,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent6">
                   <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -413,7 +413,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent5">
                   <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -439,7 +439,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
+                <a:schemeClr val="accent4">
                   <a:lumMod val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -483,9 +483,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2"/>
+                        <a:schemeClr val="accent6"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -538,9 +538,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent4"/>
+                        <a:schemeClr val="accent5"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -586,9 +586,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6"/>
+                        <a:schemeClr val="accent4"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -616,8 +616,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.562170308967596E-2"/>
-                  <c:y val="-1.2106537530266344E-2"/>
+                  <c:x val="3.7678975131876416E-2"/>
+                  <c:y val="-4.6004842615012198E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -634,9 +634,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2">
+                        <a:schemeClr val="accent6">
                           <a:lumMod val="60000"/>
                         </a:schemeClr>
                       </a:solidFill>
@@ -684,9 +684,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent4">
+                        <a:schemeClr val="accent5">
                           <a:lumMod val="60000"/>
                         </a:schemeClr>
                       </a:solidFill>
@@ -741,9 +741,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6">
+                        <a:schemeClr val="accent4">
                           <a:lumMod val="60000"/>
                         </a:schemeClr>
                       </a:solidFill>
@@ -773,8 +773,8 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.5575447570332605E-2"/>
-                  <c:y val="8.0428954423592495E-3"/>
+                  <c:x val="-1.6532466222430559E-2"/>
+                  <c:y val="7.9140531162400505E-4"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -791,9 +791,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2">
+                        <a:schemeClr val="accent6">
                           <a:lumMod val="80000"/>
                           <a:lumOff val="20000"/>
                         </a:schemeClr>
@@ -824,8 +824,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.9186134137151468E-2"/>
-                  <c:y val="0"/>
+                  <c:x val="-0.13262999246420498"/>
+                  <c:y val="-1.7756049924986721E-16"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -842,9 +842,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent4">
+                        <a:schemeClr val="accent5">
                           <a:lumMod val="80000"/>
                           <a:lumOff val="20000"/>
                         </a:schemeClr>
@@ -875,8 +875,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.3564431047475515E-2"/>
-                  <c:y val="-2.4213075060532689E-3"/>
+                  <c:x val="-4.220045214770158E-2"/>
+                  <c:y val="4.8426150121065378E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -893,9 +893,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6">
+                        <a:schemeClr val="accent4">
                           <a:lumMod val="80000"/>
                           <a:lumOff val="20000"/>
                         </a:schemeClr>
@@ -938,9 +938,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent2">
+                        <a:schemeClr val="accent6">
                           <a:lumMod val="80000"/>
                         </a:schemeClr>
                       </a:solidFill>
@@ -963,8 +963,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.17274308872656929"/>
-                      <c:h val="0.17092009685230025"/>
+                      <c:w val="0.2134363818689958"/>
+                      <c:h val="0.28956416464891038"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -977,8 +977,8 @@
               <c:idx val="10"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.3564431047475508E-2"/>
-                  <c:y val="7.2639225181598066E-3"/>
+                  <c:x val="-9.495101733232858E-2"/>
+                  <c:y val="9.6852300242130755E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -995,9 +995,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent4">
+                        <a:schemeClr val="accent5">
                           <a:lumMod val="80000"/>
                         </a:schemeClr>
                       </a:solidFill>
@@ -1045,9 +1045,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="accent6">
+                        <a:schemeClr val="accent4">
                           <a:lumMod val="80000"/>
                         </a:schemeClr>
                       </a:solidFill>
@@ -1087,7 +1087,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="accent1"/>
                     </a:solidFill>
@@ -1285,10 +1285,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
-  <a:schemeClr val="accent2"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1851,8 +1851,8 @@
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>

</xml_diff>